<commit_message>
updates - including weighted average
</commit_message>
<xml_diff>
--- a/frequency_count_GA.xlsx
+++ b/frequency_count_GA.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mraisle/Documents/OneDrive - University of North Carolina at Chapel Hill/OEF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganraisle/Documents/OEF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B579607C-7752-514B-8AA9-22BEF3982476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9490B08-6BE7-9B49-B6D3-EBB05E34D7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="1500" windowWidth="24640" windowHeight="13600"/>
+    <workbookView xWindow="560" yWindow="540" windowWidth="24640" windowHeight="13600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="frequency_count_GA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>Albany, GA</t>
   </si>
@@ -41,9 +53,6 @@
   </si>
   <si>
     <t>Tallahassee-Thomasville</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>Georgia</t>
@@ -69,11 +78,26 @@
   <si>
     <t>DMA</t>
   </si>
+  <si>
+    <t>Chattanooga</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>Columbus</t>
+  </si>
+  <si>
+    <t>Thomasville</t>
+  </si>
+  <si>
+    <t>Once week or month</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -213,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,8 +423,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -515,6 +545,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="medium">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="7"/>
+      </left>
+      <right style="thin">
+        <color theme="7"/>
+      </right>
+      <top style="thin">
+        <color theme="7"/>
+      </top>
+      <bottom style="thin">
+        <color theme="7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -560,13 +620,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -654,8 +723,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:J18" totalsRowShown="0">
-  <autoFilter ref="A12:J18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A12:J18" totalsRowShown="0">
+  <autoFilter ref="A12:J18" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -668,30 +737,28 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" name="DMA"/>
-    <tableColumn id="2" name="Albany, GA" dataDxfId="8"/>
-    <tableColumn id="3" name="Atlanta" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DMA"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Albany" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Atlanta" dataDxfId="7">
       <calculatedColumnFormula>C2/$C$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Augusta-Aiken" dataDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Augusta-Aiken" dataDxfId="6">
       <calculatedColumnFormula>D2/$D$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Columbus, GA (Opelika, AL)" dataDxfId="5">
-      <calculatedColumnFormula>E2/$E$2</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" name="Macon" dataDxfId="4">
+    <tableColumn id="12" xr3:uid="{331C4759-602C-3745-863E-4A305FEFFE97}" name="Chattanooga" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Columbus" dataDxfId="4">
       <calculatedColumnFormula>F2/$F$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Savannah" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Macon" dataDxfId="3">
       <calculatedColumnFormula>G2/$G$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Tallahassee-Thomasville" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Savannah" dataDxfId="2">
       <calculatedColumnFormula>H2/$H$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Unknown" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Thomasville" dataDxfId="1">
       <calculatedColumnFormula>I2/$I$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Georgia" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Georgia" dataDxfId="0">
       <calculatedColumnFormula>J2/$J$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -995,22 +1062,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D8:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -1024,27 +1092,27 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>17</v>
@@ -1056,27 +1124,27 @@
         <v>11</v>
       </c>
       <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
         <v>16</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>25</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>15</v>
       </c>
-      <c r="I2">
-        <v>65</v>
-      </c>
       <c r="J2">
-        <v>483</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1091,24 +1159,24 @@
         <v>3</v>
       </c>
       <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>7</v>
       </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
       <c r="J3">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -1120,27 +1188,27 @@
         <v>2</v>
       </c>
       <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>8</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>25</v>
-      </c>
       <c r="J4">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1152,27 +1220,27 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F5">
         <v>6</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1184,19 +1252,19 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>2</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
       </c>
       <c r="J6">
         <v>50</v>
@@ -1204,7 +1272,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1216,30 +1284,30 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
       <c r="J7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1247,28 +1315,28 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
         <v>4</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="I12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
         <v>7</v>
-      </c>
-      <c r="J12" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
         <v>17</v>
@@ -1280,27 +1348,27 @@
         <v>11</v>
       </c>
       <c r="E13" s="3">
+        <v>11</v>
+      </c>
+      <c r="F13" s="3">
         <v>16</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>19</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>25</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>15</v>
       </c>
-      <c r="I13" s="3">
-        <v>65</v>
-      </c>
       <c r="J13" s="3">
-        <v>483</v>
+        <v>494</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <f>B3/B2</f>
@@ -1316,32 +1384,32 @@
       </c>
       <c r="E14" s="1">
         <f>E3/$E$2</f>
-        <v>0.1875</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F14" s="1">
         <f>F3/$F$2</f>
-        <v>0.21052631578947367</v>
+        <v>0.1875</v>
       </c>
       <c r="G14" s="1">
         <f>G3/$G$2</f>
-        <v>0.4</v>
+        <v>0.21052631578947367</v>
       </c>
       <c r="H14" s="1">
         <f>H3/$H$2</f>
-        <v>0.46666666666666667</v>
+        <v>0.4</v>
       </c>
       <c r="I14" s="1">
         <f>I3/$I$2</f>
-        <v>0.18461538461538463</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="J14" s="1">
         <f>J3/$J$2</f>
-        <v>0.31469979296066253</v>
+        <v>0.31376518218623484</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1">
         <f>B4/B2</f>
@@ -1356,33 +1424,33 @@
         <v>0.18181818181818182</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:E18" si="1">E4/$E$2</f>
-        <v>0.3125</v>
+        <f t="shared" ref="E15:E17" si="1">E4/$E$2</f>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" ref="F15:F18" si="2">F4/$F$2</f>
-        <v>0.31578947368421051</v>
+        <v>0.3125</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" ref="G15:G18" si="3">G4/$G$2</f>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="H15" s="1">
+        <f>H4/$H$2</f>
         <v>0.32</v>
       </c>
-      <c r="H15" s="1">
-        <f t="shared" ref="H15:H18" si="4">H4/$H$2</f>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15:I18" si="4">I4/$I$2</f>
         <v>0.2</v>
       </c>
-      <c r="I15" s="1">
-        <f t="shared" ref="I15:I18" si="5">I4/$I$2</f>
-        <v>0.38461538461538464</v>
-      </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15:J18" si="6">J4/$J$2</f>
-        <v>0.2939958592132505</v>
+        <f t="shared" ref="J15:J18" si="5">J4/$J$2</f>
+        <v>0.29352226720647773</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <f>B5/B2</f>
@@ -1397,40 +1465,40 @@
         <v>0.27272727272727271</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.375</v>
+        <f>E5/$E$2</f>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="2"/>
-        <v>0.31578947368421051</v>
+        <v>0.375</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="3"/>
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" ref="H16:H18" si="6">H5/$H$2</f>
         <v>0.08</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <f t="shared" si="4"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <f t="shared" si="5"/>
-        <v>0.2</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="6"/>
-        <v>0.2484472049689441</v>
+        <v>0.24898785425101214</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
         <f>B6/B2</f>
         <v>0.11764705882352941</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ref="C15:C18" si="7">C6/$C$2</f>
+        <f t="shared" ref="C17:C18" si="7">C6/$C$2</f>
         <v>8.2539682539682538E-2</v>
       </c>
       <c r="D17" s="1">
@@ -1439,32 +1507,32 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="2"/>
-        <v>0.10526315789473684</v>
+        <v>0.125</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="3"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <f t="shared" si="4"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="I17" s="1">
-        <f t="shared" si="5"/>
-        <v>0.16923076923076924</v>
-      </c>
       <c r="J17" s="1">
-        <f t="shared" si="6"/>
-        <v>0.10351966873706005</v>
+        <f>J6/$J$2</f>
+        <v>0.10121457489878542</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
         <f>B7/B2</f>
@@ -1479,28 +1547,517 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>E7/$E$2</f>
+        <v>0.18181818181818182</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="2"/>
-        <v>5.2631578947368418E-2</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="H18" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
         <f t="shared" si="4"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <f t="shared" si="5"/>
-        <v>6.1538461538461542E-2</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="6"/>
-        <v>3.9337474120082816E-2</v>
+        <v>4.2510121457489877E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="8">
+        <v>17</v>
+      </c>
+      <c r="C24" s="8">
+        <v>315</v>
+      </c>
+      <c r="D24" s="8">
+        <v>11</v>
+      </c>
+      <c r="E24" s="8">
+        <v>11</v>
+      </c>
+      <c r="F24" s="8">
+        <v>16</v>
+      </c>
+      <c r="G24" s="8">
+        <v>19</v>
+      </c>
+      <c r="H24" s="8">
+        <v>25</v>
+      </c>
+      <c r="I24" s="8">
+        <v>15</v>
+      </c>
+      <c r="J24" s="8">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0.1875</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="9">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.31376518218623484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.27619047619047621</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0.29352226720647773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="E27" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.24898785425101214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="C28" s="10">
+        <v>8.2539682539682538E-2</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J28" s="10">
+        <v>0.10121457489878542</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>4.1269841269841269E-2</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0</v>
+      </c>
+      <c r="G29" s="9">
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0</v>
+      </c>
+      <c r="I29" s="9">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="J29" s="9">
+        <v>4.2510121457489877E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="8">
+        <v>315</v>
+      </c>
+      <c r="C32" s="8">
+        <v>25</v>
+      </c>
+      <c r="D32" s="8">
+        <v>19</v>
+      </c>
+      <c r="E32" s="8">
+        <v>17</v>
+      </c>
+      <c r="F32" s="8">
+        <v>16</v>
+      </c>
+      <c r="G32" s="8">
+        <v>15</v>
+      </c>
+      <c r="H32" s="8">
+        <v>11</v>
+      </c>
+      <c r="I32" s="8">
+        <v>11</v>
+      </c>
+      <c r="J32" s="8">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0.1875</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="I33" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.31376518218623484</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="10">
+        <v>0.27619047619047621</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J34" s="10">
+        <v>0.29352226720647773</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="10">
+        <f>SUM(B33:B34)</f>
+        <v>0.60952380952380958</v>
+      </c>
+      <c r="C35" s="10">
+        <f t="shared" ref="C35:J35" si="8">SUM(C33:C34)</f>
+        <v>0.72</v>
+      </c>
+      <c r="D35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="E35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.6470588235294118</v>
+      </c>
+      <c r="F35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" si="8"/>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="J35" s="10">
+        <f>SUM(J33:J34)</f>
+        <v>0.60728744939271251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="C36" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.31578947368421051</v>
+      </c>
+      <c r="E36" s="9">
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0.375</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="I36" s="9">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.24898785425101214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="10">
+        <v>8.2539682539682538E-2</v>
+      </c>
+      <c r="C37" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.10121457489878542</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="9">
+        <v>4.1269841269841269E-2</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>5.2631578947368418E-2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0</v>
+      </c>
+      <c r="G38" s="9">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0</v>
+      </c>
+      <c r="I38" s="9">
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="J38" s="9">
+        <v>4.2510121457489877E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>